<commit_message>
Minor changes in docs
</commit_message>
<xml_diff>
--- a/analyza.xlsx
+++ b/analyza.xlsx
@@ -247,7 +247,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919425E-2"/>
+          <c:x val="4.8761933643919439E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -427,8 +427,8 @@
           <c:order val="4"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -478,8 +478,9 @@
           <c:order val="5"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="75000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -529,9 +530,9 @@
           <c:order val="6"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -576,25 +577,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="101219712"/>
-        <c:axId val="101225600"/>
+        <c:axId val="109350912"/>
+        <c:axId val="109352448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101219712"/>
+        <c:axId val="109350912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="101225600"/>
+        <c:crossAx val="109352448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101225600"/>
+        <c:axId val="109352448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -622,7 +623,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="101219712"/>
+        <c:crossAx val="109350912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -650,7 +651,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919425E-2"/>
+          <c:x val="4.8761933643919439E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -1329,25 +1330,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="110764416"/>
-        <c:axId val="110765952"/>
+        <c:axId val="119522048"/>
+        <c:axId val="119523584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110764416"/>
+        <c:axId val="119522048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="110765952"/>
+        <c:crossAx val="119523584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110765952"/>
+        <c:axId val="119523584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1375,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="110764416"/>
+        <c:crossAx val="119522048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -1402,7 +1403,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919446E-2"/>
+          <c:x val="4.876193364391946E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -2068,25 +2069,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="111923968"/>
-        <c:axId val="111925504"/>
+        <c:axId val="119559296"/>
+        <c:axId val="119560832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111923968"/>
+        <c:axId val="119559296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="111925504"/>
+        <c:crossAx val="119560832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111925504"/>
+        <c:axId val="119560832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -2115,7 +2116,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="111923968"/>
+        <c:crossAx val="119559296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -2143,7 +2144,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919474E-2"/>
+          <c:x val="4.8761933643919481E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -2809,25 +2810,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="112043520"/>
-        <c:axId val="112045056"/>
+        <c:axId val="119678848"/>
+        <c:axId val="119680384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112043520"/>
+        <c:axId val="119678848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="112045056"/>
+        <c:crossAx val="119680384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112045056"/>
+        <c:axId val="119680384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="400"/>
@@ -2855,7 +2856,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="112043520"/>
+        <c:crossAx val="119678848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2882,7 +2883,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919411E-2"/>
+          <c:x val="4.8761933643919418E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -3551,25 +3552,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="113539328"/>
-        <c:axId val="113549312"/>
+        <c:axId val="120879744"/>
+        <c:axId val="120889728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113539328"/>
+        <c:axId val="120879744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="113549312"/>
+        <c:crossAx val="120889728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113549312"/>
+        <c:axId val="120889728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3596,7 +3597,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="113539328"/>
+        <c:crossAx val="120879744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -3624,7 +3625,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919425E-2"/>
+          <c:x val="4.8761933643919439E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -4296,25 +4297,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="113646592"/>
-        <c:axId val="113664768"/>
+        <c:axId val="121056640"/>
+        <c:axId val="121074816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113646592"/>
+        <c:axId val="121056640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="113664768"/>
+        <c:crossAx val="121074816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113664768"/>
+        <c:axId val="121074816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4341,7 +4342,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="113646592"/>
+        <c:crossAx val="121056640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -4369,7 +4370,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919446E-2"/>
+          <c:x val="4.876193364391946E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -5038,25 +5039,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="114138496"/>
-        <c:axId val="114148480"/>
+        <c:axId val="123588608"/>
+        <c:axId val="123590144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114138496"/>
+        <c:axId val="123588608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="114148480"/>
+        <c:crossAx val="123590144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114148480"/>
+        <c:axId val="123590144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -5085,7 +5086,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="114138496"/>
+        <c:crossAx val="123588608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -5113,7 +5114,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919474E-2"/>
+          <c:x val="4.8761933643919481E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -5782,25 +5783,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="114278784"/>
-        <c:axId val="114280320"/>
+        <c:axId val="129024768"/>
+        <c:axId val="129026304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114278784"/>
+        <c:axId val="129024768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="114280320"/>
+        <c:crossAx val="129026304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114280320"/>
+        <c:axId val="129026304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="400"/>
@@ -5828,7 +5829,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="114278784"/>
+        <c:crossAx val="129024768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5855,7 +5856,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919411E-2"/>
+          <c:x val="4.8761933643919418E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -6354,25 +6355,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="114164096"/>
-        <c:axId val="114165632"/>
+        <c:axId val="123671296"/>
+        <c:axId val="123672832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114164096"/>
+        <c:axId val="123671296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="114165632"/>
+        <c:crossAx val="123672832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114165632"/>
+        <c:axId val="123672832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6399,7 +6400,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="114164096"/>
+        <c:crossAx val="123671296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -6427,7 +6428,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919425E-2"/>
+          <c:x val="4.8761933643919439E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -6936,25 +6937,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="114455296"/>
-        <c:axId val="114456832"/>
+        <c:axId val="129201280"/>
+        <c:axId val="129202816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114455296"/>
+        <c:axId val="129201280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="114456832"/>
+        <c:crossAx val="129202816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114456832"/>
+        <c:axId val="129202816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6981,7 +6982,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="114455296"/>
+        <c:crossAx val="129201280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -7009,7 +7010,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919446E-2"/>
+          <c:x val="4.876193364391946E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -7508,25 +7509,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="114664192"/>
-        <c:axId val="114665728"/>
+        <c:axId val="129406080"/>
+        <c:axId val="129407616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114664192"/>
+        <c:axId val="129406080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="114665728"/>
+        <c:crossAx val="129407616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114665728"/>
+        <c:axId val="129407616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -7555,7 +7556,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="114664192"/>
+        <c:crossAx val="129406080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -7583,7 +7584,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919446E-2"/>
+          <c:x val="4.876193364391946E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -7766,8 +7767,8 @@
           <c:order val="4"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -7817,8 +7818,9 @@
           <c:order val="5"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="75000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -7868,9 +7870,9 @@
           <c:order val="6"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -7915,25 +7917,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="102649856"/>
-        <c:axId val="102651392"/>
+        <c:axId val="112419200"/>
+        <c:axId val="112420736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102649856"/>
+        <c:axId val="112419200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="102651392"/>
+        <c:crossAx val="112420736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102651392"/>
+        <c:axId val="112420736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7960,7 +7962,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="102649856"/>
+        <c:crossAx val="112419200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -7988,7 +7990,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919474E-2"/>
+          <c:x val="4.8761933643919481E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -8487,25 +8489,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="114689152"/>
-        <c:axId val="114690688"/>
+        <c:axId val="129435136"/>
+        <c:axId val="129436672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114689152"/>
+        <c:axId val="129435136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="114690688"/>
+        <c:crossAx val="129436672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114690688"/>
+        <c:axId val="129436672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="400"/>
@@ -8533,7 +8535,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="114689152"/>
+        <c:crossAx val="129435136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8560,7 +8562,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919446E-2"/>
+          <c:x val="4.876193364391946E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -9229,25 +9231,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="114887680"/>
-        <c:axId val="114909952"/>
+        <c:axId val="129568128"/>
+        <c:axId val="129586304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114887680"/>
+        <c:axId val="129568128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="114909952"/>
+        <c:crossAx val="129586304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114909952"/>
+        <c:axId val="129586304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -9276,7 +9278,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="114887680"/>
+        <c:crossAx val="129568128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -9304,7 +9306,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919474E-2"/>
+          <c:x val="4.8761933643919481E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -9970,25 +9972,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="115023232"/>
-        <c:axId val="115033216"/>
+        <c:axId val="129781760"/>
+        <c:axId val="129783296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115023232"/>
+        <c:axId val="129781760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="115033216"/>
+        <c:crossAx val="129783296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115033216"/>
+        <c:axId val="129783296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -10017,7 +10019,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="115023232"/>
+        <c:crossAx val="129781760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -10045,7 +10047,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919474E-2"/>
+          <c:x val="4.8761933643919481E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -10714,25 +10716,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="115225728"/>
-        <c:axId val="115227264"/>
+        <c:axId val="129910272"/>
+        <c:axId val="129911808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115225728"/>
+        <c:axId val="129910272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="115227264"/>
+        <c:crossAx val="129911808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115227264"/>
+        <c:axId val="129911808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -10761,7 +10763,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="115225728"/>
+        <c:crossAx val="129910272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -10789,7 +10791,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919474E-2"/>
+          <c:x val="4.8761933643919481E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -11288,25 +11290,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="115319552"/>
-        <c:axId val="115321088"/>
+        <c:axId val="130077824"/>
+        <c:axId val="130079360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115319552"/>
+        <c:axId val="130077824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="115321088"/>
+        <c:crossAx val="130079360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115321088"/>
+        <c:axId val="130079360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -11335,7 +11337,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="115319552"/>
+        <c:crossAx val="130077824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -11363,7 +11365,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919474E-2"/>
+          <c:x val="4.8761933643919481E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -11546,8 +11548,8 @@
           <c:order val="4"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -11597,8 +11599,9 @@
           <c:order val="5"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="75000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -11648,9 +11651,9 @@
           <c:order val="6"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -11695,25 +11698,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="105217408"/>
-        <c:axId val="105231488"/>
+        <c:axId val="112635904"/>
+        <c:axId val="112637440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="105217408"/>
+        <c:axId val="112635904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="105231488"/>
+        <c:crossAx val="112637440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105231488"/>
+        <c:axId val="112637440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -11742,7 +11745,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="105217408"/>
+        <c:crossAx val="112635904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -11770,7 +11773,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919488E-2"/>
+          <c:x val="4.8761933643919501E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -11953,8 +11956,8 @@
           <c:order val="4"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -12009,6 +12012,17 @@
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
@@ -12055,9 +12069,9 @@
           <c:order val="6"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -12102,25 +12116,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="105278464"/>
-        <c:axId val="105292544"/>
+        <c:axId val="112688512"/>
+        <c:axId val="112702592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="105278464"/>
+        <c:axId val="112688512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="105292544"/>
+        <c:crossAx val="112702592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105292544"/>
+        <c:axId val="112702592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="400"/>
@@ -12148,7 +12162,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="105278464"/>
+        <c:crossAx val="112688512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12175,7 +12189,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.876193364391939E-2"/>
+          <c:x val="4.8761933643919397E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -12844,25 +12858,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="103428480"/>
-        <c:axId val="103430016"/>
+        <c:axId val="112542464"/>
+        <c:axId val="112544000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103428480"/>
+        <c:axId val="112542464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="103430016"/>
+        <c:crossAx val="112544000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103430016"/>
+        <c:axId val="112544000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12889,7 +12903,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="103428480"/>
+        <c:crossAx val="112542464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -12917,7 +12931,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919411E-2"/>
+          <c:x val="4.8761933643919418E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -13586,25 +13600,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="105498112"/>
-        <c:axId val="105499648"/>
+        <c:axId val="118474624"/>
+        <c:axId val="118476160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="105498112"/>
+        <c:axId val="118474624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="105499648"/>
+        <c:crossAx val="118476160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105499648"/>
+        <c:axId val="118476160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13631,7 +13645,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="105498112"/>
+        <c:crossAx val="118474624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -13659,7 +13673,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919425E-2"/>
+          <c:x val="4.8761933643919439E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -14328,25 +14342,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="110102784"/>
-        <c:axId val="110112768"/>
+        <c:axId val="118545024"/>
+        <c:axId val="118555008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110102784"/>
+        <c:axId val="118545024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="110112768"/>
+        <c:crossAx val="118555008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110112768"/>
+        <c:axId val="118555008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -14375,7 +14389,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="110102784"/>
+        <c:crossAx val="118545024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -14403,7 +14417,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919446E-2"/>
+          <c:x val="4.876193364391946E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -15072,25 +15086,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="110287488"/>
-        <c:axId val="110174592"/>
+        <c:axId val="119008256"/>
+        <c:axId val="118633216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110287488"/>
+        <c:axId val="119008256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="110174592"/>
+        <c:crossAx val="118633216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110174592"/>
+        <c:axId val="118633216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15117,7 +15131,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="110287488"/>
+        <c:crossAx val="119008256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15144,7 +15158,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8761933643919411E-2"/>
+          <c:x val="4.8761933643919418E-2"/>
           <c:y val="1.9200206978018802E-2"/>
           <c:w val="0.93235857306708514"/>
           <c:h val="0.89415470926056406"/>
@@ -15810,25 +15824,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="110648320"/>
-        <c:axId val="110658304"/>
+        <c:axId val="119467392"/>
+        <c:axId val="119342208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110648320"/>
+        <c:axId val="119467392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="110658304"/>
+        <c:crossAx val="119342208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110658304"/>
+        <c:axId val="119342208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -15856,7 +15870,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="110648320"/>
+        <c:crossAx val="119467392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -24428,19 +24442,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="no-door_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="no-door" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="no-door" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="no-door_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24743,8 +24757,8 @@
   <sheetPr codeName="List1"/>
   <dimension ref="A1:P121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M117" sqref="M117"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F155" sqref="F155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28886,7 +28900,7 @@
   <sheetPr codeName="List2"/>
   <dimension ref="A1:P181"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Z213" sqref="Z213"/>
     </sheetView>
   </sheetViews>

</xml_diff>